<commit_message>
English translation of sheet names
</commit_message>
<xml_diff>
--- a/docs/howto-acdc19-nat/ACDC2019-OptAnalysesToDo.xlsx
+++ b/docs/howto-acdc19-nat/ACDC2019-OptAnalysesToDo.xlsx
@@ -5,15 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Echantillons1_impl" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Echantillons2_impl" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Modèles_impl" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="TroncaturesAuto_impl" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="TroncaturesSyst_impl" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="TroncaturesSpé_expl" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Samples1_impl" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Samples2_impl" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Models_impl" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="AutoTruncations_impl" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="SystematicTruncations_impl" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="SpecialTroncations_expl" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -253,21 +253,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="56.01"/>
   </cols>
@@ -354,7 +354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -364,11 +364,11 @@
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="7.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="107.55"/>
   </cols>
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -437,7 +437,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.44"/>
@@ -485,7 +485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -495,11 +495,11 @@
       <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="126.89"/>
   </cols>
@@ -591,21 +591,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="60.89"/>
   </cols>
@@ -697,7 +697,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -707,11 +707,11 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90234375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="95.45"/>
   </cols>

</xml_diff>